<commit_message>
UPDATE: second test has been made && TODO: optimaize and final test befor launch
</commit_message>
<xml_diff>
--- a/python-script-genesis/datos/documeto_cruce.xlsx
+++ b/python-script-genesis/datos/documeto_cruce.xlsx
@@ -994,7 +994,7 @@
         <v>18764058378338</v>
       </c>
       <c r="D11" t="n">
-        <v>1119</v>
+        <v>1137</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -1896,7 +1896,7 @@
         <v>18764056384886</v>
       </c>
       <c r="D28" t="n">
-        <v>8773</v>
+        <v>8784</v>
       </c>
       <c r="E28" t="n">
         <v>4911</v>
@@ -1925,7 +1925,7 @@
         </is>
       </c>
       <c r="K28" t="n">
-        <v>1658</v>
+        <v>1663</v>
       </c>
       <c r="L28" t="n">
         <v>1</v>
@@ -4160,7 +4160,7 @@
         <v>18764058100691</v>
       </c>
       <c r="D70" t="n">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="E70" t="n">
         <v>1</v>
@@ -5268,7 +5268,7 @@
         <v>18764051987580</v>
       </c>
       <c r="D91" t="n">
-        <v>9151</v>
+        <v>9177</v>
       </c>
       <c r="E91" t="n">
         <v>4925</v>
@@ -5748,7 +5748,7 @@
         <v>18764046461851</v>
       </c>
       <c r="D100" t="n">
-        <v>52697</v>
+        <v>52702</v>
       </c>
       <c r="E100" t="n">
         <v>50001</v>
@@ -5914,7 +5914,7 @@
         <v>18764043063912</v>
       </c>
       <c r="D103" t="n">
-        <v>4617</v>
+        <v>4619</v>
       </c>
       <c r="E103" t="n">
         <v>4000</v>
@@ -5943,7 +5943,7 @@
         </is>
       </c>
       <c r="K103" t="n">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="L103" t="n">
         <v>1</v>
@@ -6716,7 +6716,7 @@
         <v>18764052693141</v>
       </c>
       <c r="D118" t="n">
-        <v>2761</v>
+        <v>2773</v>
       </c>
       <c r="E118" t="n">
         <v>1</v>
@@ -6934,7 +6934,7 @@
         <v>18764046461851</v>
       </c>
       <c r="D122" t="n">
-        <v>53714</v>
+        <v>53729</v>
       </c>
       <c r="E122" t="n">
         <v>50001</v>
@@ -7367,27 +7367,27 @@
         <v>22366</v>
       </c>
       <c r="C130" t="n">
-        <v>18764018580234</v>
+        <v>18764004701439</v>
       </c>
       <c r="D130" t="n">
-        <v>6380</v>
+        <v>3684</v>
       </c>
       <c r="E130" t="n">
-        <v>3695</v>
+        <v>1</v>
       </c>
       <c r="F130" t="n">
         <v>10000</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
+          <t>25/09/2020 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
           <t>25/09/2021 12:00:00 a. m.</t>
         </is>
       </c>
-      <c r="H130" t="inlineStr">
-        <is>
-          <t>25/09/2022 12:00:00 a. m.</t>
-        </is>
-      </c>
       <c r="I130" t="inlineStr">
         <is>
           <t>FEC1</t>
@@ -7399,7 +7399,7 @@
         </is>
       </c>
       <c r="K130" t="n">
-        <v>301</v>
+        <v>151</v>
       </c>
       <c r="L130" t="n">
         <v>1</v>
@@ -7417,25 +7417,25 @@
         <v>22366</v>
       </c>
       <c r="C131" t="n">
-        <v>18764004701439</v>
+        <v>18764018580234</v>
       </c>
       <c r="D131" t="n">
-        <v>3684</v>
+        <v>6380</v>
       </c>
       <c r="E131" t="n">
-        <v>1</v>
+        <v>3695</v>
       </c>
       <c r="F131" t="n">
         <v>10000</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>25/09/2020 12:00:00 a. m.</t>
+          <t>25/09/2021 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>25/09/2021 12:00:00 a. m.</t>
+          <t>25/09/2022 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="I131" t="inlineStr">
@@ -7449,7 +7449,7 @@
         </is>
       </c>
       <c r="K131" t="n">
-        <v>151</v>
+        <v>301</v>
       </c>
       <c r="L131" t="n">
         <v>1</v>
@@ -7470,7 +7470,7 @@
         <v>18764058658147</v>
       </c>
       <c r="D132" t="n">
-        <v>9697</v>
+        <v>9715</v>
       </c>
       <c r="E132" t="n">
         <v>8300</v>
@@ -8276,7 +8276,7 @@
         <v>18764043229395</v>
       </c>
       <c r="D147" t="n">
-        <v>3757</v>
+        <v>3771</v>
       </c>
       <c r="E147" t="n">
         <v>1</v>
@@ -8330,7 +8330,7 @@
         <v>18764057890669</v>
       </c>
       <c r="D148" t="n">
-        <v>5362</v>
+        <v>5372</v>
       </c>
       <c r="E148" t="n">
         <v>4521</v>
@@ -9934,7 +9934,7 @@
         <v>18764053718565</v>
       </c>
       <c r="D178" t="n">
-        <v>21237</v>
+        <v>21253</v>
       </c>
       <c r="E178" t="n">
         <v>19085</v>
@@ -9963,7 +9963,7 @@
         </is>
       </c>
       <c r="K178" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L178" t="n">
         <v>1</v>
@@ -10408,7 +10408,7 @@
         <v>18764058369886</v>
       </c>
       <c r="D187" t="n">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E187" t="n">
         <v>1</v>
@@ -11048,7 +11048,7 @@
         <v>18764057174807</v>
       </c>
       <c r="D199" t="n">
-        <v>1213</v>
+        <v>1242</v>
       </c>
       <c r="E199" t="n">
         <v>1</v>
@@ -11077,7 +11077,7 @@
         </is>
       </c>
       <c r="K199" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L199" t="n">
         <v>1</v>
@@ -11505,7 +11505,7 @@
         </is>
       </c>
       <c r="K207" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L207" t="n">
         <v>1</v>
@@ -11742,7 +11742,7 @@
         <v>18764055945693</v>
       </c>
       <c r="D212" t="n">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="E212" t="n">
         <v>1</v>
@@ -15054,7 +15054,7 @@
         <v>18764046809200</v>
       </c>
       <c r="D274" t="n">
-        <v>12551</v>
+        <v>12560</v>
       </c>
       <c r="E274" t="n">
         <v>5001</v>
@@ -16580,7 +16580,7 @@
         <v>18764056656292</v>
       </c>
       <c r="D303" t="n">
-        <v>6902</v>
+        <v>6920</v>
       </c>
       <c r="E303" t="n">
         <v>5442</v>
@@ -16788,7 +16788,7 @@
         <v>18764047466756</v>
       </c>
       <c r="D307" t="n">
-        <v>6837</v>
+        <v>6857</v>
       </c>
       <c r="E307" t="n">
         <v>1</v>
@@ -17480,7 +17480,7 @@
         <v>18764055949514</v>
       </c>
       <c r="D320" t="n">
-        <v>10447</v>
+        <v>10466</v>
       </c>
       <c r="E320" t="n">
         <v>8216</v>
@@ -17509,7 +17509,7 @@
         </is>
       </c>
       <c r="K320" t="n">
-        <v>1668</v>
+        <v>1678</v>
       </c>
       <c r="L320" t="n">
         <v>1</v>
@@ -18690,7 +18690,7 @@
         <v>18764056095415</v>
       </c>
       <c r="D343" t="n">
-        <v>8151</v>
+        <v>8162</v>
       </c>
       <c r="E343" t="n">
         <v>6667</v>
@@ -19214,7 +19214,7 @@
         <v>18764056231933</v>
       </c>
       <c r="D353" t="n">
-        <v>1668</v>
+        <v>1680</v>
       </c>
       <c r="E353" t="n">
         <v>1</v>
@@ -20672,7 +20672,7 @@
         <v>18764044482716</v>
       </c>
       <c r="D380" t="n">
-        <v>7487</v>
+        <v>7511</v>
       </c>
       <c r="E380" t="n">
         <v>1</v>
@@ -21820,7 +21820,7 @@
         <v>18764056487425</v>
       </c>
       <c r="D402" t="n">
-        <v>11262</v>
+        <v>11313</v>
       </c>
       <c r="E402" t="n">
         <v>9179</v>
@@ -21849,7 +21849,7 @@
         </is>
       </c>
       <c r="K402" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L402" t="n">
         <v>1</v>
@@ -22606,7 +22606,7 @@
         <v>18764053318571</v>
       </c>
       <c r="D417" t="n">
-        <v>18716</v>
+        <v>18742</v>
       </c>
       <c r="E417" t="n">
         <v>15181</v>
@@ -22635,7 +22635,7 @@
         </is>
       </c>
       <c r="K417" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L417" t="n">
         <v>1</v>
@@ -23966,7 +23966,7 @@
         <v>18764052163411</v>
       </c>
       <c r="D443" t="n">
-        <v>2309</v>
+        <v>2316</v>
       </c>
       <c r="E443" t="n">
         <v>1001</v>
@@ -26240,7 +26240,7 @@
         <v>18764049665737</v>
       </c>
       <c r="D486" t="n">
-        <v>52641</v>
+        <v>52671</v>
       </c>
       <c r="E486" t="n">
         <v>45001</v>
@@ -26399,25 +26399,25 @@
         <v>61171</v>
       </c>
       <c r="C489" t="n">
-        <v>18764016322974</v>
+        <v>18764003139511</v>
       </c>
       <c r="D489" t="n">
-        <v>20001</v>
+        <v>17514</v>
       </c>
       <c r="E489" t="n">
-        <v>17495</v>
+        <v>10001</v>
       </c>
       <c r="F489" t="n">
         <v>20000</v>
       </c>
       <c r="G489" t="inlineStr">
         <is>
-          <t>12/08/2021 12:00:00 a. m.</t>
+          <t>27/08/2020 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="H489" t="inlineStr">
         <is>
-          <t>12/08/2022 12:00:00 a. m.</t>
+          <t>27/08/2021 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="I489" t="inlineStr">
@@ -26431,7 +26431,7 @@
         </is>
       </c>
       <c r="K489" t="n">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="L489" t="n">
         <v>1</v>
@@ -26449,25 +26449,25 @@
         <v>61171</v>
       </c>
       <c r="C490" t="n">
-        <v>18764003139511</v>
+        <v>18764016322974</v>
       </c>
       <c r="D490" t="n">
-        <v>17514</v>
+        <v>20001</v>
       </c>
       <c r="E490" t="n">
-        <v>10001</v>
+        <v>17495</v>
       </c>
       <c r="F490" t="n">
         <v>20000</v>
       </c>
       <c r="G490" t="inlineStr">
         <is>
-          <t>27/08/2020 12:00:00 a. m.</t>
+          <t>12/08/2021 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="H490" t="inlineStr">
         <is>
-          <t>27/08/2021 12:00:00 a. m.</t>
+          <t>12/08/2022 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="I490" t="inlineStr">
@@ -26481,7 +26481,7 @@
         </is>
       </c>
       <c r="K490" t="n">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="L490" t="n">
         <v>1</v>
@@ -26610,7 +26610,7 @@
         <v>18764033871657</v>
       </c>
       <c r="D493" t="n">
-        <v>18262</v>
+        <v>12270</v>
       </c>
       <c r="E493" t="n">
         <v>12195</v>
@@ -26664,7 +26664,7 @@
         <v>18764033871657</v>
       </c>
       <c r="D494" t="n">
-        <v>12270</v>
+        <v>18262</v>
       </c>
       <c r="E494" t="n">
         <v>12195</v>
@@ -27188,7 +27188,7 @@
         <v>18764062323720</v>
       </c>
       <c r="D504" t="n">
-        <v>30249</v>
+        <v>30273</v>
       </c>
       <c r="E504" t="n">
         <v>30001</v>
@@ -27217,7 +27217,7 @@
         </is>
       </c>
       <c r="K504" t="n">
-        <v>1332</v>
+        <v>1334</v>
       </c>
       <c r="L504" t="n">
         <v>1</v>
@@ -28342,7 +28342,7 @@
         <v>18764054191012</v>
       </c>
       <c r="D526" t="n">
-        <v>6747</v>
+        <v>6766</v>
       </c>
       <c r="E526" t="n">
         <v>2534</v>
@@ -30334,7 +30334,7 @@
         <v>18764056754210</v>
       </c>
       <c r="D564" t="n">
-        <v>12431</v>
+        <v>12442</v>
       </c>
       <c r="E564" t="n">
         <v>10927</v>
@@ -31278,7 +31278,7 @@
         <v>18764058396309</v>
       </c>
       <c r="D582" t="n">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="E582" t="n">
         <v>558</v>
@@ -31307,7 +31307,7 @@
         </is>
       </c>
       <c r="K582" t="n">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="L582" t="n">
         <v>1</v>
@@ -32134,7 +32134,7 @@
         <v>18764055601157</v>
       </c>
       <c r="D598" t="n">
-        <v>6986</v>
+        <v>6997</v>
       </c>
       <c r="E598" t="n">
         <v>5158</v>
@@ -32816,7 +32816,7 @@
         <v>18764062535354</v>
       </c>
       <c r="D611" t="n">
-        <v>1922</v>
+        <v>1931</v>
       </c>
       <c r="E611" t="n">
         <v>1869</v>
@@ -32845,7 +32845,7 @@
         </is>
       </c>
       <c r="K611" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L611" t="n">
         <v>1</v>
@@ -33348,7 +33348,7 @@
         <v>18764057065553</v>
       </c>
       <c r="D621" t="n">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="E621" t="n">
         <v>986</v>
@@ -34974,7 +34974,7 @@
         <v>18764055771176</v>
       </c>
       <c r="D652" t="n">
-        <v>31570</v>
+        <v>31592</v>
       </c>
       <c r="E652" t="n">
         <v>30001</v>
@@ -35003,7 +35003,7 @@
         </is>
       </c>
       <c r="K652" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L652" t="n">
         <v>1</v>

</xml_diff>